<commit_message>
finalizando o desafio final
</commit_message>
<xml_diff>
--- a/desafio_final_relatorio.xlsx
+++ b/desafio_final_relatorio.xlsx
@@ -2515,7 +2515,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C127"/>
+  <dimension ref="A1:C163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4176,6 +4176,474 @@
       </c>
       <c r="C127" t="n">
         <v>3751</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>701</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>claro</t>
+        </is>
+      </c>
+      <c r="C128" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>701</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>oi</t>
+        </is>
+      </c>
+      <c r="C129" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>701</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>tim</t>
+        </is>
+      </c>
+      <c r="C130" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>701</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>vivo</t>
+        </is>
+      </c>
+      <c r="C131" t="n">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>610</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>claro</t>
+        </is>
+      </c>
+      <c r="C132" t="n">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>610</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>oi</t>
+        </is>
+      </c>
+      <c r="C133" t="n">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>610</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>tim</t>
+        </is>
+      </c>
+      <c r="C134" t="n">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>610</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>vivo</t>
+        </is>
+      </c>
+      <c r="C135" t="n">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>609</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>claro</t>
+        </is>
+      </c>
+      <c r="C136" t="n">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>609</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>oi</t>
+        </is>
+      </c>
+      <c r="C137" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>609</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>tim</t>
+        </is>
+      </c>
+      <c r="C138" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>609</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>vivo</t>
+        </is>
+      </c>
+      <c r="C139" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>201</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>claro</t>
+        </is>
+      </c>
+      <c r="C140" t="n">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>201</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>oi</t>
+        </is>
+      </c>
+      <c r="C141" t="n">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>201</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>tim</t>
+        </is>
+      </c>
+      <c r="C142" t="n">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>201</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>vivo</t>
+        </is>
+      </c>
+      <c r="C143" t="n">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>202</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>claro</t>
+        </is>
+      </c>
+      <c r="C144" t="n">
+        <v>2399</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>202</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>oi</t>
+        </is>
+      </c>
+      <c r="C145" t="n">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>202</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>tim</t>
+        </is>
+      </c>
+      <c r="C146" t="n">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>202</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>vivo</t>
+        </is>
+      </c>
+      <c r="C147" t="n">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>206</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>claro</t>
+        </is>
+      </c>
+      <c r="C148" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>206</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>oi</t>
+        </is>
+      </c>
+      <c r="C149" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>206</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>vivo</t>
+        </is>
+      </c>
+      <c r="C150" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>613</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>claro</t>
+        </is>
+      </c>
+      <c r="C151" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>613</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>oi</t>
+        </is>
+      </c>
+      <c r="C152" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>613</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>tim</t>
+        </is>
+      </c>
+      <c r="C153" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>613</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>vivo</t>
+        </is>
+      </c>
+      <c r="C154" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>616</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>claro</t>
+        </is>
+      </c>
+      <c r="C155" t="n">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>616</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>oi</t>
+        </is>
+      </c>
+      <c r="C156" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>616</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>tim</t>
+        </is>
+      </c>
+      <c r="C157" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>616</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>vivo</t>
+        </is>
+      </c>
+      <c r="C158" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>205</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>claro</t>
+        </is>
+      </c>
+      <c r="C159" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>401</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>claro</t>
+        </is>
+      </c>
+      <c r="C160" t="n">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>401</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>oi</t>
+        </is>
+      </c>
+      <c r="C161" t="n">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>401</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>tim</t>
+        </is>
+      </c>
+      <c r="C162" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>401</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>vivo</t>
+        </is>
+      </c>
+      <c r="C163" t="n">
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -5413,11 +5881,11 @@
         <v>1585</v>
       </c>
       <c r="D58" t="n">
-        <v>0</v>
+        <v>1585</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -5434,11 +5902,11 @@
         <v>634</v>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>634</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -5455,11 +5923,11 @@
         <v>520</v>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>520</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -5476,11 +5944,11 @@
         <v>521</v>
       </c>
       <c r="D61" t="n">
-        <v>0</v>
+        <v>521</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -5497,11 +5965,11 @@
         <v>2399</v>
       </c>
       <c r="D62" t="n">
-        <v>0</v>
+        <v>2399</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -5518,11 +5986,11 @@
         <v>602</v>
       </c>
       <c r="D63" t="n">
-        <v>0</v>
+        <v>602</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -5539,11 +6007,11 @@
         <v>310</v>
       </c>
       <c r="D64" t="n">
-        <v>0</v>
+        <v>310</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -5560,11 +6028,11 @@
         <v>447</v>
       </c>
       <c r="D65" t="n">
-        <v>0</v>
+        <v>447</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -5581,11 +6049,11 @@
         <v>123</v>
       </c>
       <c r="D66" t="n">
-        <v>0</v>
+        <v>123</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -5602,11 +6070,11 @@
         <v>45</v>
       </c>
       <c r="D67" t="n">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -5623,11 +6091,11 @@
         <v>40</v>
       </c>
       <c r="D68" t="n">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -5644,11 +6112,11 @@
         <v>15</v>
       </c>
       <c r="D69" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -5665,11 +6133,11 @@
         <v>500</v>
       </c>
       <c r="D70" t="n">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -5686,11 +6154,11 @@
         <v>375</v>
       </c>
       <c r="D71" t="n">
-        <v>0</v>
+        <v>375</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -5707,11 +6175,11 @@
         <v>125</v>
       </c>
       <c r="D72" t="n">
-        <v>0</v>
+        <v>125</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -5728,11 +6196,11 @@
         <v>343</v>
       </c>
       <c r="D73" t="n">
-        <v>0</v>
+        <v>343</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -6736,11 +7204,11 @@
         <v>486</v>
       </c>
       <c r="D121" t="n">
-        <v>0</v>
+        <v>486</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -6757,11 +7225,11 @@
         <v>90</v>
       </c>
       <c r="D122" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -6778,11 +7246,11 @@
         <v>90</v>
       </c>
       <c r="D123" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -6799,11 +7267,11 @@
         <v>60</v>
       </c>
       <c r="D124" t="n">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -6820,11 +7288,11 @@
         <v>260</v>
       </c>
       <c r="D125" t="n">
-        <v>0</v>
+        <v>260</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -6841,11 +7309,11 @@
         <v>135</v>
       </c>
       <c r="D126" t="n">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -6862,11 +7330,11 @@
         <v>540</v>
       </c>
       <c r="D127" t="n">
-        <v>0</v>
+        <v>540</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -6883,11 +7351,11 @@
         <v>1400</v>
       </c>
       <c r="D128" t="n">
-        <v>0</v>
+        <v>1400</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -7072,11 +7540,11 @@
         <v>90</v>
       </c>
       <c r="D137" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -7093,7 +7561,7 @@
         <v>84</v>
       </c>
       <c r="D138" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -7114,7 +7582,7 @@
         <v>50</v>
       </c>
       <c r="D139" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -7135,11 +7603,11 @@
         <v>35</v>
       </c>
       <c r="D140" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -7324,7 +7792,7 @@
         <v>426</v>
       </c>
       <c r="D149" t="n">
-        <v>0</v>
+        <v>411</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -7345,11 +7813,11 @@
         <v>95</v>
       </c>
       <c r="D150" t="n">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -7366,11 +7834,11 @@
         <v>50</v>
       </c>
       <c r="D151" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -7387,11 +7855,11 @@
         <v>70</v>
       </c>
       <c r="D152" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -7576,11 +8044,11 @@
         <v>140</v>
       </c>
       <c r="D161" t="n">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -7597,11 +8065,11 @@
         <v>20</v>
       </c>
       <c r="D162" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -7618,11 +8086,11 @@
         <v>135</v>
       </c>
       <c r="D163" t="n">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>
@@ -7639,11 +8107,11 @@
         <v>304</v>
       </c>
       <c r="D164" t="n">
-        <v>0</v>
+        <v>304</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
-          <t>Alerta</t>
+          <t>ok</t>
         </is>
       </c>
     </row>

</xml_diff>